<commit_message>
Adding new function to process text in class
</commit_message>
<xml_diff>
--- a/src/data/amlo_labeling.xlsx
+++ b/src/data/amlo_labeling.xlsx
@@ -4,10 +4,10 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Hoja 2"/>
+    <sheet r:id="rId1" sheetId="1" name="labels"/>
     <sheet r:id="rId2" sheetId="2" name="frases_odio"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
@@ -1088,7 +1088,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1121,10 +1121,10 @@
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -1152,6 +1152,9 @@
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1460,36 +1463,36 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="13" width="51.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="22" width="51.71928571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="22" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="26" max="26" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="22" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="22" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="22" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="22" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="22" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="22" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="22" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="22" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="22" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="22" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="22" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="22" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="22" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="22" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="22" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="22" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="22" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="22" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="22" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="22" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="26" max="26" style="22" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -1986,7 +1989,7 @@
       <c r="Y13" s="17"/>
       <c r="Z13" s="17"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="45.75">
       <c r="A14" s="4">
         <v>20211011</v>
       </c>
@@ -2024,7 +2027,7 @@
       <c r="Y14" s="17"/>
       <c r="Z14" s="17"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="45.75">
       <c r="A15" s="4">
         <v>20190430</v>
       </c>
@@ -2062,7 +2065,7 @@
       <c r="Y15" s="17"/>
       <c r="Z15" s="17"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="45.75">
       <c r="A16" s="4">
         <v>20220603</v>
       </c>
@@ -2100,7 +2103,7 @@
       <c r="Y16" s="17"/>
       <c r="Z16" s="17"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="45.75">
       <c r="A17" s="4">
         <v>20211223</v>
       </c>
@@ -2138,7 +2141,7 @@
       <c r="Y17" s="17"/>
       <c r="Z17" s="17"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="45.75">
       <c r="A18" s="4">
         <v>20200128</v>
       </c>
@@ -2176,7 +2179,7 @@
       <c r="Y18" s="17"/>
       <c r="Z18" s="17"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="45.75">
       <c r="A19" s="4">
         <v>20210324</v>
       </c>
@@ -2214,7 +2217,7 @@
       <c r="Y19" s="17"/>
       <c r="Z19" s="17"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="45.75">
       <c r="A20" s="4">
         <v>20210810</v>
       </c>
@@ -2252,7 +2255,7 @@
       <c r="Y20" s="17"/>
       <c r="Z20" s="17"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="45.75">
       <c r="A21" s="4">
         <v>20231023</v>
       </c>
@@ -2290,7 +2293,7 @@
       <c r="Y21" s="17"/>
       <c r="Z21" s="17"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="45.75">
       <c r="A22" s="4">
         <v>20191218</v>
       </c>
@@ -29972,7 +29975,7 @@
   </sheetPr>
   <dimension ref="A1:C1064"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>